<commit_message>
command and adapter working
</commit_message>
<xml_diff>
--- a/genReport/xlsxD.xlsx
+++ b/genReport/xlsxD.xlsx
@@ -15,7 +15,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+  <si>
+    <t>omar</t>
+  </si>
+  <si>
+    <t>1997-05-31</t>
+  </si>
+  <si>
+    <t>omar@gmail.com</t>
+  </si>
+  <si>
+    <t>7110eda4d09e062aa5e4a390b0a572ac0d2c0220</t>
+  </si>
+  <si>
+    <t>01157979606</t>
+  </si>
+  <si>
+    <t>Mo</t>
+  </si>
+  <si>
+    <t>2000-05-31</t>
+  </si>
+  <si>
+    <t>mo@gmail.com</t>
+  </si>
+  <si>
+    <t>ac1ab23d6288711be64a25bf13432baf1e60b2bd</t>
+  </si>
+  <si>
+    <t>012825347698</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,14 +380,73 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>